<commit_message>
Fixing issues with wrong union on child creation
</commit_message>
<xml_diff>
--- a/tests/fixtures_files/fs-PotenteAsegurado.xlsx
+++ b/tests/fixtures_files/fs-PotenteAsegurado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
   <si>
     <t xml:space="preserve">offset=0 count=20 +surname:potente~ +mother_givenname:andrea~ +mother_surname:asegurado~ +record_country:Spain </t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>ark:/61903/1:1:FFMD-XJC</t>
+  </si>
+  <si>
+    <t>test_capture_notknow</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -305,7 +311,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -417,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AA20"/>
+  <dimension ref="A2:AB20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -731,20 +737,20 @@
     <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -803,31 +809,34 @@
         <v>20</v>
       </c>
       <c r="T6" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" t="s">
         <v>21</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>22</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>23</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>24</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -852,17 +861,17 @@
       <c r="Q7" t="s">
         <v>35</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>36</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>37</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="AA7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -884,17 +893,20 @@
       <c r="Q8" t="s">
         <v>35</v>
       </c>
-      <c r="V8" t="s">
+      <c r="T8" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" t="s">
         <v>36</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>37</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="AA8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -922,17 +934,17 @@
       <c r="Q9" t="s">
         <v>35</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>36</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>37</v>
       </c>
-      <c r="Z9" s="6" t="s">
+      <c r="AA9" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -960,17 +972,17 @@
       <c r="Q10" t="s">
         <v>35</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>36</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>37</v>
       </c>
-      <c r="Z10" s="7" t="s">
+      <c r="AA10" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -995,17 +1007,17 @@
       <c r="Q11" t="s">
         <v>35</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>36</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>37</v>
       </c>
-      <c r="Z11" s="8" t="s">
+      <c r="AA11" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1030,17 +1042,17 @@
       <c r="Q12" t="s">
         <v>35</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>36</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>37</v>
       </c>
-      <c r="Z12" s="9" t="s">
+      <c r="AA12" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1071,17 +1083,17 @@
       <c r="Q13" t="s">
         <v>35</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>61</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>37</v>
       </c>
-      <c r="Z13" s="10" t="s">
+      <c r="AA13" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1112,17 +1124,17 @@
       <c r="Q14" t="s">
         <v>35</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>61</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>37</v>
       </c>
-      <c r="Z14" s="11" t="s">
+      <c r="AA14" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1156,17 +1168,17 @@
       <c r="Q15" t="s">
         <v>35</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>61</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>37</v>
       </c>
-      <c r="Z15" s="12" t="s">
+      <c r="AA15" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1197,17 +1209,17 @@
       <c r="Q16" t="s">
         <v>35</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>61</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="13" t="s">
+      <c r="AA16" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1238,17 +1250,17 @@
       <c r="Q17" t="s">
         <v>35</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>61</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>37</v>
       </c>
-      <c r="Z17" s="14" t="s">
+      <c r="AA17" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1279,17 +1291,17 @@
       <c r="Q18" t="s">
         <v>35</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>61</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>37</v>
       </c>
-      <c r="Z18" s="15" t="s">
+      <c r="AA18" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1320,17 +1332,17 @@
       <c r="Q19" t="s">
         <v>35</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>61</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>37</v>
       </c>
-      <c r="Z19" s="16" t="s">
+      <c r="AA19" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>6.4099998474121094</v>
       </c>
@@ -1361,34 +1373,34 @@
       <c r="Q20" t="s">
         <v>35</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>61</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>37</v>
       </c>
-      <c r="Z20" s="17" t="s">
+      <c r="AA20" s="17" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="url"/>
-    <hyperlink ref="Z6" r:id="rId2" display="url"/>
-    <hyperlink ref="Z7" r:id="rId3" display="url"/>
-    <hyperlink ref="Z8" r:id="rId4" display="url"/>
-    <hyperlink ref="Z9" r:id="rId5" display="url"/>
-    <hyperlink ref="Z10" r:id="rId6" display="url"/>
-    <hyperlink ref="Z11" r:id="rId7" display="url"/>
-    <hyperlink ref="Z12" r:id="rId8" display="url"/>
-    <hyperlink ref="Z13" r:id="rId9" display="url"/>
-    <hyperlink ref="Z14" r:id="rId10" display="url"/>
-    <hyperlink ref="Z15" r:id="rId11" display="url"/>
-    <hyperlink ref="Z16" r:id="rId12" display="url"/>
-    <hyperlink ref="Z17" r:id="rId13" display="url"/>
-    <hyperlink ref="Z18" r:id="rId14" display="url"/>
-    <hyperlink ref="Z19" r:id="rId15" display="url"/>
-    <hyperlink ref="Z20" r:id="rId16" display="url"/>
+    <hyperlink ref="A2" r:id="rId1" location="&amp;offset=0&amp;count=20&amp;query=+surname:potente~ +mother_givenname:andrea~ +mother_surname:asegurado~ +record_country:Spain" display="url"/>
+    <hyperlink ref="AA6" r:id="rId2" display="url"/>
+    <hyperlink ref="AA7" r:id="rId3" display="url"/>
+    <hyperlink ref="AA8" r:id="rId4" display="url"/>
+    <hyperlink ref="AA9" r:id="rId5" display="url"/>
+    <hyperlink ref="AA10" r:id="rId6" display="url"/>
+    <hyperlink ref="AA11" r:id="rId7" display="url"/>
+    <hyperlink ref="AA12" r:id="rId8" display="url"/>
+    <hyperlink ref="AA13" r:id="rId9" display="url"/>
+    <hyperlink ref="AA14" r:id="rId10" display="url"/>
+    <hyperlink ref="AA15" r:id="rId11" display="url"/>
+    <hyperlink ref="AA16" r:id="rId12" display="url"/>
+    <hyperlink ref="AA17" r:id="rId13" display="url"/>
+    <hyperlink ref="AA18" r:id="rId14" display="url"/>
+    <hyperlink ref="AA19" r:id="rId15" display="url"/>
+    <hyperlink ref="AA20" r:id="rId16" display="url"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>